<commit_message>
-- added xlsx states and counties
</commit_message>
<xml_diff>
--- a/inst/extdata/FEMA/NRI/NRIDataDictionary.xlsx
+++ b/inst/extdata/FEMA/NRI/NRIDataDictionary.xlsx
@@ -3935,11 +3935,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I480"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="A445" sqref="A445:XFD469"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="2" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
@@ -5228,7 +5228,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="67" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6011,7 +6011,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6417,7 +6417,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6446,7 +6446,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="89" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6562,7 +6562,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6591,7 +6591,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6649,7 +6649,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6852,7 +6852,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6910,7 +6910,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6939,7 +6939,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>104</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>105</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>106</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>107</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>108</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>109</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>110</v>
       </c>
@@ -7171,7 +7171,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>111</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>112</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>113</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="115" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" s="2" customFormat="1" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>115</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>116</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>117</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>118</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>119</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>120</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>121</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>122</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>123</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>124</v>
       </c>
@@ -7577,7 +7577,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>125</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>126</v>
       </c>
@@ -7635,7 +7635,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>127</v>
       </c>
@@ -7664,7 +7664,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>128</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>129</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="131" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>131</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>132</v>
       </c>
@@ -7809,7 +7809,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>133</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>134</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>135</v>
       </c>
@@ -7896,7 +7896,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>136</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>137</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>138</v>
       </c>
@@ -7983,7 +7983,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>139</v>
       </c>
@@ -8012,7 +8012,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>140</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>141</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>142</v>
       </c>
@@ -8099,7 +8099,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>143</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>144</v>
       </c>
@@ -8157,7 +8157,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>145</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>146</v>
       </c>
@@ -8215,7 +8215,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>147</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>148</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>149</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>150</v>
       </c>
@@ -8331,7 +8331,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>151</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="153" spans="1:9" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" s="2" customFormat="1" ht="12.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -8389,7 +8389,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>153</v>
       </c>
@@ -8418,7 +8418,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>154</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>155</v>
       </c>
@@ -8476,7 +8476,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>156</v>
       </c>
@@ -8505,7 +8505,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>157</v>
       </c>
@@ -8534,7 +8534,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>158</v>
       </c>
@@ -8563,7 +8563,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>159</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>160</v>
       </c>
@@ -8621,7 +8621,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>161</v>
       </c>
@@ -8650,7 +8650,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>162</v>
       </c>
@@ -8679,7 +8679,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>163</v>
       </c>
@@ -8708,7 +8708,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>164</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>165</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>166</v>
       </c>
@@ -8795,7 +8795,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>167</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>168</v>
       </c>
@@ -8853,7 +8853,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>169</v>
       </c>
@@ -8882,7 +8882,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>170</v>
       </c>
@@ -8911,7 +8911,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>171</v>
       </c>
@@ -8940,7 +8940,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>172</v>
       </c>
@@ -8969,7 +8969,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>173</v>
       </c>
@@ -8998,7 +8998,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>174</v>
       </c>
@@ -9027,7 +9027,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>175</v>
       </c>
@@ -9056,7 +9056,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>176</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>177</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="179" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -9143,7 +9143,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>179</v>
       </c>
@@ -9172,7 +9172,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>180</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>181</v>
       </c>
@@ -9230,7 +9230,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>182</v>
       </c>
@@ -9259,7 +9259,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>183</v>
       </c>
@@ -9288,7 +9288,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>184</v>
       </c>
@@ -9317,7 +9317,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>185</v>
       </c>
@@ -9346,7 +9346,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>186</v>
       </c>
@@ -9375,7 +9375,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>187</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>188</v>
       </c>
@@ -9433,7 +9433,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>189</v>
       </c>
@@ -9462,7 +9462,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>190</v>
       </c>
@@ -9491,7 +9491,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>191</v>
       </c>
@@ -9520,7 +9520,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>192</v>
       </c>
@@ -9549,7 +9549,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>193</v>
       </c>
@@ -9578,7 +9578,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>194</v>
       </c>
@@ -9607,7 +9607,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>195</v>
       </c>
@@ -9636,7 +9636,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>196</v>
       </c>
@@ -9665,7 +9665,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>197</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>198</v>
       </c>
@@ -9723,7 +9723,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>199</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>200</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>201</v>
       </c>
@@ -9810,7 +9810,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>202</v>
       </c>
@@ -9839,7 +9839,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>203</v>
       </c>
@@ -9868,7 +9868,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="205" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:9" s="2" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -9897,7 +9897,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>205</v>
       </c>
@@ -9926,7 +9926,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>206</v>
       </c>
@@ -9955,7 +9955,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>207</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>208</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>209</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>210</v>
       </c>
@@ -10071,7 +10071,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>211</v>
       </c>
@@ -10100,7 +10100,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>212</v>
       </c>
@@ -10129,7 +10129,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>213</v>
       </c>
@@ -10158,7 +10158,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>214</v>
       </c>
@@ -10187,7 +10187,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>215</v>
       </c>
@@ -10216,7 +10216,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>216</v>
       </c>
@@ -10245,7 +10245,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>217</v>
       </c>
@@ -10274,7 +10274,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>218</v>
       </c>
@@ -10303,7 +10303,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>219</v>
       </c>
@@ -10332,7 +10332,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>220</v>
       </c>
@@ -10361,7 +10361,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>221</v>
       </c>
@@ -10390,7 +10390,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>222</v>
       </c>
@@ -10419,7 +10419,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>223</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>224</v>
       </c>
@@ -10477,7 +10477,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>225</v>
       </c>
@@ -10506,7 +10506,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>226</v>
       </c>
@@ -10535,7 +10535,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>227</v>
       </c>
@@ -10564,7 +10564,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>228</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="231" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A231" s="2">
         <v>230</v>
       </c>
@@ -10651,7 +10651,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>231</v>
       </c>
@@ -10680,7 +10680,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>232</v>
       </c>
@@ -10709,7 +10709,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>233</v>
       </c>
@@ -10738,7 +10738,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>234</v>
       </c>
@@ -10767,7 +10767,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>235</v>
       </c>
@@ -10796,7 +10796,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>236</v>
       </c>
@@ -10825,7 +10825,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>237</v>
       </c>
@@ -10854,7 +10854,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>238</v>
       </c>
@@ -10883,7 +10883,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>239</v>
       </c>
@@ -10912,7 +10912,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>240</v>
       </c>
@@ -10941,7 +10941,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>241</v>
       </c>
@@ -10970,7 +10970,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>242</v>
       </c>
@@ -10999,7 +10999,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>243</v>
       </c>
@@ -11028,7 +11028,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>244</v>
       </c>
@@ -11057,7 +11057,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>245</v>
       </c>
@@ -11086,7 +11086,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>246</v>
       </c>
@@ -11115,7 +11115,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>247</v>
       </c>
@@ -11144,7 +11144,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>248</v>
       </c>
@@ -11173,7 +11173,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>249</v>
       </c>
@@ -11202,7 +11202,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>250</v>
       </c>
@@ -11231,7 +11231,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>251</v>
       </c>
@@ -11260,7 +11260,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="253" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A253" s="2">
         <v>252</v>
       </c>
@@ -11289,7 +11289,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A254">
         <v>253</v>
       </c>
@@ -11318,7 +11318,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A255">
         <v>254</v>
       </c>
@@ -11347,7 +11347,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A256">
         <v>255</v>
       </c>
@@ -11376,7 +11376,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A257">
         <v>256</v>
       </c>
@@ -11405,7 +11405,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A258">
         <v>257</v>
       </c>
@@ -11434,7 +11434,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A259">
         <v>258</v>
       </c>
@@ -11463,7 +11463,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A260">
         <v>259</v>
       </c>
@@ -11492,7 +11492,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A261">
         <v>260</v>
       </c>
@@ -11521,7 +11521,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A262">
         <v>261</v>
       </c>
@@ -11550,7 +11550,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A263">
         <v>262</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A264">
         <v>263</v>
       </c>
@@ -11608,7 +11608,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A265">
         <v>264</v>
       </c>
@@ -11637,7 +11637,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A266">
         <v>265</v>
       </c>
@@ -11666,7 +11666,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A267">
         <v>266</v>
       </c>
@@ -11695,7 +11695,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A268">
         <v>267</v>
       </c>
@@ -11724,7 +11724,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A269">
         <v>268</v>
       </c>
@@ -11753,7 +11753,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A270">
         <v>269</v>
       </c>
@@ -11782,7 +11782,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A271">
         <v>270</v>
       </c>
@@ -11811,7 +11811,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A272">
         <v>271</v>
       </c>
@@ -11840,7 +11840,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A273">
         <v>272</v>
       </c>
@@ -11869,7 +11869,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A274">
         <v>273</v>
       </c>
@@ -11898,7 +11898,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="275" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A275" s="2">
         <v>274</v>
       </c>
@@ -11927,7 +11927,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A276">
         <v>275</v>
       </c>
@@ -11956,7 +11956,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A277">
         <v>276</v>
       </c>
@@ -11985,7 +11985,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A278">
         <v>277</v>
       </c>
@@ -12014,7 +12014,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A279">
         <v>278</v>
       </c>
@@ -12043,7 +12043,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A280">
         <v>279</v>
       </c>
@@ -12072,7 +12072,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A281">
         <v>280</v>
       </c>
@@ -12101,7 +12101,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A282">
         <v>281</v>
       </c>
@@ -12130,7 +12130,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A283">
         <v>282</v>
       </c>
@@ -12159,7 +12159,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A284">
         <v>283</v>
       </c>
@@ -12188,7 +12188,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A285">
         <v>284</v>
       </c>
@@ -12217,7 +12217,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A286">
         <v>285</v>
       </c>
@@ -12246,7 +12246,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A287">
         <v>286</v>
       </c>
@@ -12275,7 +12275,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A288">
         <v>287</v>
       </c>
@@ -12304,7 +12304,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A289">
         <v>288</v>
       </c>
@@ -12333,7 +12333,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A290">
         <v>289</v>
       </c>
@@ -12362,7 +12362,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A291">
         <v>290</v>
       </c>
@@ -12391,7 +12391,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A292">
         <v>291</v>
       </c>
@@ -12420,7 +12420,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A293">
         <v>292</v>
       </c>
@@ -12449,7 +12449,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A294">
         <v>293</v>
       </c>
@@ -12478,7 +12478,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A295">
         <v>294</v>
       </c>
@@ -12507,7 +12507,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A296">
         <v>295</v>
       </c>
@@ -12536,7 +12536,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="297" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A297" s="2">
         <v>296</v>
       </c>
@@ -12565,7 +12565,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A298">
         <v>297</v>
       </c>
@@ -12594,7 +12594,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A299">
         <v>298</v>
       </c>
@@ -12623,7 +12623,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A300">
         <v>299</v>
       </c>
@@ -12652,7 +12652,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A301">
         <v>300</v>
       </c>
@@ -12681,7 +12681,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A302">
         <v>301</v>
       </c>
@@ -12710,7 +12710,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A303">
         <v>302</v>
       </c>
@@ -12739,7 +12739,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A304">
         <v>303</v>
       </c>
@@ -12768,7 +12768,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A305">
         <v>304</v>
       </c>
@@ -12797,7 +12797,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A306">
         <v>305</v>
       </c>
@@ -12826,7 +12826,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A307">
         <v>306</v>
       </c>
@@ -12855,7 +12855,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A308">
         <v>307</v>
       </c>
@@ -12884,7 +12884,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A309">
         <v>308</v>
       </c>
@@ -12913,7 +12913,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A310">
         <v>309</v>
       </c>
@@ -12942,7 +12942,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A311">
         <v>310</v>
       </c>
@@ -12971,7 +12971,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A312">
         <v>311</v>
       </c>
@@ -13000,7 +13000,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A313">
         <v>312</v>
       </c>
@@ -13029,7 +13029,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A314">
         <v>313</v>
       </c>
@@ -13058,7 +13058,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A315">
         <v>314</v>
       </c>
@@ -13087,7 +13087,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A316">
         <v>315</v>
       </c>
@@ -13116,7 +13116,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A317">
         <v>316</v>
       </c>
@@ -13145,7 +13145,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A318">
         <v>317</v>
       </c>
@@ -13174,7 +13174,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A319">
         <v>318</v>
       </c>
@@ -13203,7 +13203,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A320">
         <v>319</v>
       </c>
@@ -13232,7 +13232,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A321">
         <v>320</v>
       </c>
@@ -13261,7 +13261,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A322">
         <v>321</v>
       </c>
@@ -13290,7 +13290,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="323" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A323" s="2">
         <v>322</v>
       </c>
@@ -13319,7 +13319,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A324">
         <v>323</v>
       </c>
@@ -13348,7 +13348,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A325">
         <v>324</v>
       </c>
@@ -13377,7 +13377,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A326">
         <v>325</v>
       </c>
@@ -13406,7 +13406,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A327">
         <v>326</v>
       </c>
@@ -13435,7 +13435,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A328">
         <v>327</v>
       </c>
@@ -13464,7 +13464,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A329">
         <v>328</v>
       </c>
@@ -13493,7 +13493,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A330">
         <v>329</v>
       </c>
@@ -13522,7 +13522,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A331">
         <v>330</v>
       </c>
@@ -13551,7 +13551,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A332">
         <v>331</v>
       </c>
@@ -13580,7 +13580,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A333">
         <v>332</v>
       </c>
@@ -13609,7 +13609,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A334">
         <v>333</v>
       </c>
@@ -13638,7 +13638,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A335">
         <v>334</v>
       </c>
@@ -13667,7 +13667,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="336" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A336">
         <v>335</v>
       </c>
@@ -13696,7 +13696,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A337">
         <v>336</v>
       </c>
@@ -13725,7 +13725,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A338">
         <v>337</v>
       </c>
@@ -13754,7 +13754,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A339">
         <v>338</v>
       </c>
@@ -13783,7 +13783,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A340">
         <v>339</v>
       </c>
@@ -13812,7 +13812,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A341">
         <v>340</v>
       </c>
@@ -13841,7 +13841,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A342">
         <v>341</v>
       </c>
@@ -13870,7 +13870,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A343">
         <v>342</v>
       </c>
@@ -13899,7 +13899,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A344">
         <v>343</v>
       </c>
@@ -13928,7 +13928,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A345">
         <v>344</v>
       </c>
@@ -13957,7 +13957,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A346">
         <v>345</v>
       </c>
@@ -13986,7 +13986,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A347">
         <v>346</v>
       </c>
@@ -14015,7 +14015,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A348">
         <v>347</v>
       </c>
@@ -14044,7 +14044,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="349" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A349" s="2">
         <v>348</v>
       </c>
@@ -14073,7 +14073,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A350">
         <v>349</v>
       </c>
@@ -14102,7 +14102,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A351">
         <v>350</v>
       </c>
@@ -14131,7 +14131,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A352">
         <v>351</v>
       </c>
@@ -14160,7 +14160,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="353" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A353">
         <v>352</v>
       </c>
@@ -14189,7 +14189,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="354" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A354">
         <v>353</v>
       </c>
@@ -14218,7 +14218,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="355" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A355">
         <v>354</v>
       </c>
@@ -14247,7 +14247,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="356" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A356">
         <v>355</v>
       </c>
@@ -14276,7 +14276,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="357" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A357">
         <v>356</v>
       </c>
@@ -14305,7 +14305,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="358" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A358">
         <v>357</v>
       </c>
@@ -14334,7 +14334,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="359" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A359">
         <v>358</v>
       </c>
@@ -14363,7 +14363,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="360" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A360">
         <v>359</v>
       </c>
@@ -14392,7 +14392,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="361" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A361">
         <v>360</v>
       </c>
@@ -14421,7 +14421,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="362" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A362">
         <v>361</v>
       </c>
@@ -14450,7 +14450,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="363" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A363">
         <v>362</v>
       </c>
@@ -14479,7 +14479,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="364" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A364">
         <v>363</v>
       </c>
@@ -14508,7 +14508,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="365" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A365">
         <v>364</v>
       </c>
@@ -14537,7 +14537,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A366">
         <v>365</v>
       </c>
@@ -14566,7 +14566,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="367" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A367">
         <v>366</v>
       </c>
@@ -14595,7 +14595,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A368">
         <v>367</v>
       </c>
@@ -14624,7 +14624,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A369">
         <v>368</v>
       </c>
@@ -14653,7 +14653,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A370">
         <v>369</v>
       </c>
@@ -14682,7 +14682,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A371">
         <v>370</v>
       </c>
@@ -14711,7 +14711,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A372">
         <v>371</v>
       </c>
@@ -14740,7 +14740,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A373">
         <v>372</v>
       </c>
@@ -14769,7 +14769,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A374">
         <v>373</v>
       </c>
@@ -14798,7 +14798,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="375" spans="1:9" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:9" s="2" customFormat="1" ht="13.5" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A375" s="2">
         <v>374</v>
       </c>
@@ -14827,7 +14827,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A376">
         <v>375</v>
       </c>
@@ -14856,7 +14856,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A377">
         <v>376</v>
       </c>
@@ -14885,7 +14885,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A378">
         <v>377</v>
       </c>
@@ -14914,7 +14914,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A379">
         <v>378</v>
       </c>
@@ -14943,7 +14943,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A380">
         <v>379</v>
       </c>
@@ -14972,7 +14972,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A381">
         <v>380</v>
       </c>
@@ -15001,7 +15001,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A382">
         <v>381</v>
       </c>
@@ -15030,7 +15030,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A383">
         <v>382</v>
       </c>
@@ -15059,7 +15059,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="384" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A384">
         <v>383</v>
       </c>
@@ -15088,7 +15088,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="385" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A385">
         <v>384</v>
       </c>
@@ -15117,7 +15117,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="386" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A386">
         <v>385</v>
       </c>
@@ -15146,7 +15146,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="387" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A387">
         <v>386</v>
       </c>
@@ -15175,7 +15175,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="388" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="388" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A388">
         <v>387</v>
       </c>
@@ -15204,7 +15204,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="389" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A389">
         <v>388</v>
       </c>
@@ -15233,7 +15233,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="390" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A390">
         <v>389</v>
       </c>
@@ -15262,7 +15262,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="391" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A391">
         <v>390</v>
       </c>
@@ -15291,7 +15291,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A392">
         <v>391</v>
       </c>
@@ -15320,7 +15320,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A393">
         <v>392</v>
       </c>
@@ -15349,7 +15349,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="394" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A394">
         <v>393</v>
       </c>
@@ -15378,7 +15378,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="395" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:9" hidden="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A395">
         <v>394</v>
       </c>
@@ -15407,7 +15407,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="396" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A396">
         <v>395</v>
       </c>
@@ -15436,7 +15436,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="397" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A397" s="2">
         <v>396</v>
       </c>
@@ -15465,7 +15465,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="398" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A398">
         <v>397</v>
       </c>
@@ -15494,7 +15494,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="399" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A399">
         <v>398</v>
       </c>
@@ -15523,7 +15523,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="400" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A400">
         <v>399</v>
       </c>
@@ -15552,7 +15552,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A401">
         <v>400</v>
       </c>
@@ -15581,7 +15581,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="402" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A402">
         <v>401</v>
       </c>
@@ -15610,7 +15610,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A403">
         <v>402</v>
       </c>
@@ -15639,7 +15639,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="404" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="404" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A404">
         <v>403</v>
       </c>
@@ -15668,7 +15668,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A405">
         <v>404</v>
       </c>
@@ -15697,7 +15697,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A406">
         <v>405</v>
       </c>
@@ -15726,7 +15726,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A407">
         <v>406</v>
       </c>
@@ -15755,7 +15755,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="408" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="408" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A408">
         <v>407</v>
       </c>
@@ -15784,7 +15784,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="409" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="409" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A409">
         <v>408</v>
       </c>
@@ -15813,7 +15813,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="410" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="410" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A410">
         <v>409</v>
       </c>
@@ -15842,7 +15842,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="411" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="411" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A411">
         <v>410</v>
       </c>
@@ -15871,7 +15871,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="412" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A412">
         <v>411</v>
       </c>
@@ -15900,7 +15900,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="413" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A413">
         <v>412</v>
       </c>
@@ -15929,7 +15929,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="414" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="414" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A414">
         <v>413</v>
       </c>
@@ -15958,7 +15958,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="415" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="415" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A415">
         <v>414</v>
       </c>
@@ -15987,7 +15987,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="416" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="416" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A416">
         <v>415</v>
       </c>
@@ -16016,7 +16016,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="417" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A417">
         <v>416</v>
       </c>
@@ -16045,7 +16045,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="418" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="418" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A418">
         <v>417</v>
       </c>
@@ -16074,7 +16074,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="419" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A419" s="2">
         <v>418</v>
       </c>
@@ -16103,7 +16103,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="420" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A420">
         <v>419</v>
       </c>
@@ -16132,7 +16132,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="421" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A421">
         <v>420</v>
       </c>
@@ -16161,7 +16161,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="422" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A422">
         <v>421</v>
       </c>
@@ -16190,7 +16190,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="423" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A423">
         <v>422</v>
       </c>
@@ -16219,7 +16219,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="424" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A424">
         <v>423</v>
       </c>
@@ -16248,7 +16248,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="425" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A425">
         <v>424</v>
       </c>
@@ -16277,7 +16277,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="426" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A426">
         <v>425</v>
       </c>
@@ -16306,7 +16306,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="427" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A427">
         <v>426</v>
       </c>
@@ -16335,7 +16335,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="428" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A428">
         <v>427</v>
       </c>
@@ -16364,7 +16364,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="429" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A429">
         <v>428</v>
       </c>
@@ -16393,7 +16393,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="430" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="430" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A430">
         <v>429</v>
       </c>
@@ -16422,7 +16422,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="431" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A431">
         <v>430</v>
       </c>
@@ -16451,7 +16451,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="432" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="432" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A432">
         <v>431</v>
       </c>
@@ -16480,7 +16480,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="433" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="433" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A433">
         <v>432</v>
       </c>
@@ -16509,7 +16509,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="434" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="434" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A434">
         <v>433</v>
       </c>
@@ -16538,7 +16538,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="435" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="435" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A435">
         <v>434</v>
       </c>
@@ -16567,7 +16567,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="436" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="436" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A436">
         <v>435</v>
       </c>
@@ -16596,7 +16596,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="437" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="437" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A437">
         <v>436</v>
       </c>
@@ -16625,7 +16625,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="438" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="438" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A438">
         <v>437</v>
       </c>
@@ -16654,7 +16654,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="439" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="439" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A439">
         <v>438</v>
       </c>
@@ -16683,7 +16683,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="440" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="440" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A440">
         <v>439</v>
       </c>
@@ -16712,7 +16712,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="441" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="441" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A441">
         <v>440</v>
       </c>
@@ -16741,7 +16741,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="442" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="442" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A442">
         <v>441</v>
       </c>
@@ -16770,7 +16770,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="443" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="443" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A443">
         <v>442</v>
       </c>
@@ -16799,7 +16799,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="444" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="444" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A444">
         <v>443</v>
       </c>
@@ -16828,7 +16828,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="445" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="445" spans="1:9" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A445" s="2">
         <v>444</v>
       </c>
@@ -16857,7 +16857,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="446" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="446" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A446">
         <v>445</v>
       </c>
@@ -16886,7 +16886,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="447" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="447" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A447">
         <v>446</v>
       </c>
@@ -16915,7 +16915,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="448" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="448" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A448">
         <v>447</v>
       </c>
@@ -16944,7 +16944,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="449" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="449" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A449">
         <v>448</v>
       </c>
@@ -16973,7 +16973,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="450" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="450" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A450">
         <v>449</v>
       </c>
@@ -17002,7 +17002,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="451" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="451" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A451">
         <v>450</v>
       </c>
@@ -17031,7 +17031,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="452" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="452" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A452">
         <v>451</v>
       </c>
@@ -17060,7 +17060,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="453" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="453" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A453">
         <v>452</v>
       </c>
@@ -17089,7 +17089,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="454" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="454" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A454">
         <v>453</v>
       </c>
@@ -17118,7 +17118,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="455" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="455" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A455">
         <v>454</v>
       </c>
@@ -17147,7 +17147,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="456" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="456" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A456">
         <v>455</v>
       </c>
@@ -17176,7 +17176,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="457" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="457" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A457">
         <v>456</v>
       </c>
@@ -17205,7 +17205,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="458" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="458" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A458">
         <v>457</v>
       </c>
@@ -17234,7 +17234,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="459" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="459" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A459">
         <v>458</v>
       </c>
@@ -17263,7 +17263,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="460" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="460" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A460">
         <v>459</v>
       </c>
@@ -17292,7 +17292,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="461" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="461" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A461">
         <v>460</v>
       </c>
@@ -17321,7 +17321,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="462" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="462" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A462">
         <v>461</v>
       </c>
@@ -17350,7 +17350,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="463" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="463" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A463">
         <v>462</v>
       </c>
@@ -17379,7 +17379,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="464" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="464" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A464">
         <v>463</v>
       </c>
@@ -17408,7 +17408,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="465" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="465" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A465">
         <v>464</v>
       </c>
@@ -17437,7 +17437,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="466" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="466" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A466">
         <v>465</v>
       </c>
@@ -17466,7 +17466,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="467" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="467" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A467">
         <v>466</v>
       </c>
@@ -17495,7 +17495,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="468" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="468" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A468">
         <v>467</v>
       </c>
@@ -17524,7 +17524,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="469" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="469" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A469">
         <v>468</v>
       </c>
@@ -17553,7 +17553,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="470" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="470" spans="1:9" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A470">
         <v>469</v>
       </c>

</xml_diff>

<commit_message>
-- added states data.table
</commit_message>
<xml_diff>
--- a/inst/extdata/FEMA/NRI/NRIDataDictionary.xlsx
+++ b/inst/extdata/FEMA/NRI/NRIDataDictionary.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NRIDataDictionary!$A$1:$I$480</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -3935,8 +3935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A445" sqref="A445:XFD469"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="B205" sqref="B205:B226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="2" x14ac:dyDescent="0.45"/>

</xml_diff>